<commit_message>
Added OK button data
Button data should now be complete for the Acer TV (1363) setting
</commit_message>
<xml_diff>
--- a/remotecodes.xlsx
+++ b/remotecodes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
   <si>
     <t>Mute</t>
   </si>
@@ -252,6 +252,15 @@
   </si>
   <si>
     <t>data 2</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>5F</t>
   </si>
 </sst>
 </file>
@@ -623,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,119 +954,130 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B31" s="3">
         <v>78</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C31" s="4">
         <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C33" s="4">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C34" s="4">
         <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="3">
-        <v>38</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>72</v>
+        <v>21</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>73</v>
+        <v>19</v>
+      </c>
+      <c r="B36" s="3">
+        <v>38</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>